<commit_message>
Figured out how to import and use my CSV!!
Now to manipulate it!
</commit_message>
<xml_diff>
--- a/Demo Sales Data.xlsx
+++ b/Demo Sales Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Not PC\Documents\GitHub\SalesReporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89065B60-485B-4E15-82B6-764D150A3E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A5DAE9-159C-458A-A2B1-6242E4B54D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="11556" windowHeight="6000" xr2:uid="{4E1C05E6-CAC8-4EBC-929A-09CBE59D1408}"/>
+    <workbookView xWindow="1068" yWindow="1068" windowWidth="11556" windowHeight="6000" xr2:uid="{4E1C05E6-CAC8-4EBC-929A-09CBE59D1408}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>Salesperson</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>Jingleheimerschmidt</t>
+  </si>
+  <si>
+    <t>Revenue</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9B4742-7E4C-4F61-BB65-595A06D643C9}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -417,18 +419,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>43831</v>
@@ -442,7 +444,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>43862</v>
@@ -456,7 +458,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>43891</v>
@@ -470,7 +472,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>43922</v>
@@ -484,7 +486,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>43952</v>
@@ -498,7 +500,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>43983</v>
@@ -512,7 +514,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>43831</v>
@@ -526,7 +528,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>43862</v>
@@ -540,7 +542,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
         <v>43891</v>
@@ -554,7 +556,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <v>43922</v>
@@ -568,7 +570,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1">
         <v>43952</v>
@@ -582,7 +584,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1">
         <v>43983</v>
@@ -596,7 +598,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1">
         <v>43831</v>
@@ -610,7 +612,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>43862</v>
@@ -624,7 +626,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>43891</v>
@@ -638,7 +640,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1">
         <v>43922</v>
@@ -652,7 +654,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="1">
         <v>43952</v>
@@ -666,7 +668,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>43983</v>

</xml_diff>

<commit_message>
Having lots of import trouble....
</commit_message>
<xml_diff>
--- a/Demo Sales Data.xlsx
+++ b/Demo Sales Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Not PC\Documents\GitHub\SalesReporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A5DAE9-159C-458A-A2B1-6242E4B54D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A861C4D-3084-4659-89E6-3F426B8E9886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="1068" windowWidth="11556" windowHeight="6000" xr2:uid="{4E1C05E6-CAC8-4EBC-929A-09CBE59D1408}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demo Sales Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -39,6 +26,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Revenue</t>
   </si>
   <si>
     <t>Cost</t>
@@ -52,15 +42,12 @@
   <si>
     <t>Jingleheimerschmidt</t>
   </si>
-  <si>
-    <t>Revenue</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +55,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -85,16 +372,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,34 +882,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F9B4742-7E4C-4F61-BB65-595A06D643C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="8.83984375" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
         <v>43831</v>
       </c>
       <c r="C2">
@@ -443,10 +923,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
         <v>43862</v>
       </c>
       <c r="C3">
@@ -457,10 +937,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
         <v>43891</v>
       </c>
       <c r="C4">
@@ -471,52 +951,52 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
         <v>43922</v>
       </c>
       <c r="C5">
         <v>110</v>
       </c>
       <c r="D5">
-        <v>93.3333333333333</v>
+        <v>93.333333330000002</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
         <v>43952</v>
       </c>
       <c r="C6">
         <v>115</v>
       </c>
       <c r="D6">
-        <v>95.8333333333333</v>
+        <v>95.833333330000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
         <v>43983</v>
       </c>
       <c r="C7">
         <v>120</v>
       </c>
       <c r="D7">
-        <v>98.3333333333333</v>
+        <v>98.333333330000002</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
         <v>43831</v>
       </c>
       <c r="C8">
@@ -527,10 +1007,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
         <v>43862</v>
       </c>
       <c r="C9">
@@ -541,66 +1021,66 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
         <v>43891</v>
       </c>
       <c r="C10">
-        <v>80.357142857142804</v>
+        <v>80.357142859999996</v>
       </c>
       <c r="D10">
-        <v>74.910714285714306</v>
+        <v>74.910714290000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
         <v>43922</v>
       </c>
       <c r="C11">
-        <v>76.547619047618994</v>
+        <v>76.547619049999994</v>
       </c>
       <c r="D11">
-        <v>72.321428571428598</v>
+        <v>72.321428569999995</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
         <v>43952</v>
       </c>
       <c r="C12">
-        <v>72.738095238095198</v>
+        <v>72.738095240000007</v>
       </c>
       <c r="D12">
-        <v>69.732142857142904</v>
+        <v>69.732142859999996</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
         <v>43983</v>
       </c>
       <c r="C13">
-        <v>68.928571428571402</v>
+        <v>68.928571430000005</v>
       </c>
       <c r="D13">
-        <v>67.142857142857096</v>
+        <v>67.142857140000004</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
         <v>43831</v>
       </c>
       <c r="C14">
@@ -611,10 +1091,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
         <v>43862</v>
       </c>
       <c r="C15">
@@ -625,59 +1105,59 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
         <v>43891</v>
       </c>
       <c r="C16">
-        <v>149.28257456828899</v>
+        <v>149.2825746</v>
       </c>
       <c r="D16">
-        <v>82.662872841444297</v>
+        <v>82.662872840000006</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
         <v>43922</v>
       </c>
       <c r="C17">
-        <v>154.44814233385699</v>
+        <v>154.4481423</v>
       </c>
       <c r="D17">
-        <v>82.335949764521203</v>
+        <v>82.335949760000005</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2">
         <v>43952</v>
       </c>
       <c r="C18">
-        <v>159.613710099424</v>
+        <v>159.61371009999999</v>
       </c>
       <c r="D18">
-        <v>82.009026687598094</v>
+        <v>82.009026689999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2">
         <v>43983</v>
       </c>
       <c r="C19">
-        <v>164.779277864992</v>
+        <v>164.77927790000001</v>
       </c>
       <c r="D19">
-        <v>81.682103610675</v>
+        <v>81.682103609999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel seems like the best way to go
</commit_message>
<xml_diff>
--- a/Demo Sales Data.xlsx
+++ b/Demo Sales Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Not PC\Documents\GitHub\SalesReporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A861C4D-3084-4659-89E6-3F426B8E9886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F108AD45-8156-4528-9441-4E0670A3AC00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="6432" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo Sales Data" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
-  <si>
-    <t>Salesperson</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
   <si>
     <t>John</t>
   </si>
@@ -46,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -882,11 +870,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -898,265 +886,251 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="B1" s="2">
+        <v>43831</v>
+      </c>
+      <c r="C1">
+        <v>100</v>
+      </c>
+      <c r="D1">
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D2">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C3">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>43891</v>
+        <v>43922</v>
       </c>
       <c r="C4">
         <v>110</v>
       </c>
       <c r="D4">
-        <v>95</v>
+        <v>93.333333330000002</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>43922</v>
+        <v>43952</v>
       </c>
       <c r="C5">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D5">
-        <v>93.333333330000002</v>
+        <v>95.833333330000002</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C6">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D6">
-        <v>95.833333330000002</v>
+        <v>98.333333330000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>43983</v>
+        <v>43831</v>
       </c>
       <c r="C7">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="D7">
-        <v>98.333333330000002</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C9">
-        <v>60</v>
+        <v>80.357142859999996</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>74.910714290000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2">
-        <v>43891</v>
+        <v>43922</v>
       </c>
       <c r="C10">
-        <v>80.357142859999996</v>
+        <v>76.547619049999994</v>
       </c>
       <c r="D10">
-        <v>74.910714290000001</v>
+        <v>72.321428569999995</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2">
-        <v>43922</v>
+        <v>43952</v>
       </c>
       <c r="C11">
-        <v>76.547619049999994</v>
+        <v>72.738095240000007</v>
       </c>
       <c r="D11">
-        <v>72.321428569999995</v>
+        <v>69.732142859999996</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C12">
-        <v>72.738095240000007</v>
+        <v>68.928571430000005</v>
       </c>
       <c r="D12">
-        <v>69.732142859999996</v>
+        <v>67.142857140000004</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
-        <v>43983</v>
+        <v>43831</v>
       </c>
       <c r="C13">
-        <v>68.928571430000005</v>
+        <v>250</v>
       </c>
       <c r="D13">
-        <v>67.142857140000004</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2">
-        <v>43831</v>
+        <v>43862</v>
       </c>
       <c r="C14">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="D14">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" s="2">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C15">
-        <v>219</v>
+        <v>149.2825746</v>
       </c>
       <c r="D15">
-        <v>90</v>
+        <v>82.662872840000006</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B16" s="2">
-        <v>43891</v>
+        <v>43922</v>
       </c>
       <c r="C16">
-        <v>149.2825746</v>
+        <v>154.4481423</v>
       </c>
       <c r="D16">
-        <v>82.662872840000006</v>
+        <v>82.335949760000005</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2">
-        <v>43922</v>
+        <v>43952</v>
       </c>
       <c r="C17">
-        <v>154.4481423</v>
+        <v>159.61371009999999</v>
       </c>
       <c r="D17">
-        <v>82.335949760000005</v>
+        <v>82.009026689999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C18">
-        <v>159.61371009999999</v>
+        <v>164.77927790000001</v>
       </c>
       <c r="D18">
-        <v>82.009026689999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2">
-        <v>43983</v>
-      </c>
-      <c r="C19">
-        <v>164.77927790000001</v>
-      </c>
-      <c r="D19">
         <v>81.682103609999999</v>
       </c>
     </row>

</xml_diff>